<commit_message>
fixed yarn scripts to build sample.xlsx directly so that it runs out of the box; added posts example where XLSX files can be used to run a simple CMS
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeddee/tmp/vuepress-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEED863-3847-AF4A-BEB7-A273622B0C50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F89DD9-99DB-3940-8F48-0B68D3BD7AE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{AA5F12E1-6ABB-5E4A-B60F-3E0D6BB9CFBA}"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{AA5F12E1-6ABB-5E4A-B60F-3E0D6BB9CFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="name this however you want" sheetId="1" r:id="rId1"/>
-    <sheet name="🎉" sheetId="2" r:id="rId2"/>
+    <sheet name="posts" sheetId="3" r:id="rId2"/>
+    <sheet name="🎉" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>column1</t>
   </si>
@@ -53,6 +54,45 @@
   </si>
   <si>
     <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>Subhead</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Getting started</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>Internediate</t>
+  </si>
+  <si>
+    <t>More information</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
+  <si>
+    <t>Part 3</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Wrapping up</t>
   </si>
 </sst>
 </file>
@@ -406,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC5C711-1677-C34D-97B3-EEDB1ACFD325}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -458,6 +498,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950FCD81-2DC2-E54C-B9A2-2B08352D656E}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544A4FA0-57A1-FE48-B997-7F2378E5AB94}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>